<commit_message>
Trying to resolve the issue with deployment on poirot
</commit_message>
<xml_diff>
--- a/ColFusionServerBLL/src/test/resources/chiaTestExcelTwoSheets.xlsx
+++ b/ColFusionServerBLL/src/test/resources/chiaTestExcelTwoSheets.xlsx
@@ -8,10 +8,10 @@
   </bookViews>
   <sheets>
     <sheet name="CHIA Level 1 Metadata Summary" sheetId="1" r:id="rId1"/>
-    <sheet name="Mortality_Madras,India_1916-21" sheetId="2" r:id="rId2"/>
+    <sheet name="Test_Test,Test_1916-21" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Mortality_Madras,India_1916-21'!$A$1:$G$1945</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Test_Test,Test_1916-21'!$A$1:$G$1945</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'CHIA Level 1 Metadata Summary'!$A$3:$C$26</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>

</xml_diff>